<commit_message>
Add a new demo: Precomputed Atmosphere Rendering
</commit_message>
<xml_diff>
--- a/docs/每日学习总结.xlsx
+++ b/docs/每日学习总结.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\StudioProjects\PostProcessingWork\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A2592B-2A4F-41A7-9B46-DFB12DCBCCD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661FE5A1-BDCA-45A8-B8BE-41391358DD2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -183,6 +183,14 @@
   </si>
   <si>
     <t>一点想法：在做Ray-marching的过程中，是否可以把直线路径当作t，而内积分的函数当作关于t的函数，再利用曲线微分几何的一些性质来快速求解积分。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>充分理解在屏幕空间计算纹理LOD的原理：需要结合微积分教材第1066页推导雅可比的过程来理解，尤其是斜边向量的定义，这是算法的关键解。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要认真的思考算法细节，尤其是数学层面的东西</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -521,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -661,6 +669,17 @@
         <v>22</v>
       </c>
     </row>
+    <row r="13" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44012</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add a new demo: FfxSssr
</commit_message>
<xml_diff>
--- a/docs/每日学习总结.xlsx
+++ b/docs/每日学习总结.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\StudioProjects\PostProcessingWork\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC45794-CBFC-4408-A155-9BEBB095541E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D006B0-BD2D-4DB5-A13F-F4E839957BA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -204,6 +204,27 @@
   </si>
   <si>
     <t>1,充分理解函数F(x,y,z)=K为什么是曲面，因为无约束的函数F(x,y,z)随着变量适当变化可能会填满整个三维空间。当函数F(x,y,z)=k存在约束时，会在空间中形成一个曲面. 2, 理解拉格朗日乘数的几何意义:当函数F(x,y,z)在约束曲面的G(x,y,z)=K变化时，F(x,y,z)也可能是一个曲面，因为(x,y,z)的值约束在有界域中.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1，贝塞尔矩形曲面F(u,v)，当u,v任意一个变量是常量时，得到的曲线均为贝塞尔曲线。
+2，贝塞尔曲线的细分算法指的是将一条贝塞尔曲线从中间拆分成两条贝塞尔曲线，然后对子曲线做常数离散化
+3，贝塞尔矩形曲面的细分算法类似，将一片曲面拆分成四个子曲面
+4，贝塞尔三角曲面与控制点所构成的三角形的直观理解不足，因此对这种方式的细分算法也不太能理解，需要更深入的研究。
+5，贝塞尔曲线曲面可以使用古典微分几何分析，并且所有的定理均适用
+6，上述的贝塞尔也可以替换成你spline或其它连续曲线曲面的名称。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量点乘不满足结合律</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1，图形学就像数学应用题：提出问题，然后根据定理、命题和推论解出问题，但是不告诉你应用了哪些定理、命题和推论。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1，图形学研究方向：构建自己的科学体系，发展出一门专门服务于图形学自身的学科，明确问题、解决过程和结果。从而约束研究人员和工程师的研究方向，节约成本和增大产出。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -542,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -712,6 +733,38 @@
         <v>27</v>
       </c>
     </row>
+    <row r="16" spans="1:4" ht="124.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44127</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44148</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44155</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>